<commit_message>
Correçoes e fiz mais bugs
</commit_message>
<xml_diff>
--- a/Barbara/Barbara_update.xlsx
+++ b/Barbara/Barbara_update.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1762" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="481">
   <si>
     <t>ID Animal</t>
   </si>
@@ -72,121 +72,124 @@
     <t>Distancia (de carro,em min) a HEFMV</t>
   </si>
   <si>
+    <t>71543</t>
+  </si>
+  <si>
+    <t>63613</t>
+  </si>
+  <si>
+    <t>32426</t>
+  </si>
+  <si>
+    <t>44144</t>
+  </si>
+  <si>
+    <t>73897</t>
+  </si>
+  <si>
+    <t>28090</t>
+  </si>
+  <si>
+    <t>59891</t>
+  </si>
+  <si>
     <t>9511</t>
   </si>
   <si>
-    <t>32426</t>
-  </si>
-  <si>
-    <t>44144</t>
-  </si>
-  <si>
-    <t>63613</t>
-  </si>
-  <si>
-    <t>59891</t>
-  </si>
-  <si>
-    <t>71543</t>
-  </si>
-  <si>
-    <t>73897</t>
-  </si>
-  <si>
-    <t>28090</t>
-  </si>
-  <si>
     <t>69455</t>
   </si>
   <si>
     <t>33556</t>
   </si>
   <si>
+    <t>3343</t>
+  </si>
+  <si>
     <t>45317</t>
   </si>
   <si>
-    <t>3343</t>
+    <t>57307</t>
+  </si>
+  <si>
+    <t>52909</t>
   </si>
   <si>
     <t>20095</t>
   </si>
   <si>
+    <t>74753</t>
+  </si>
+  <si>
+    <t>73634</t>
+  </si>
+  <si>
+    <t>72002</t>
+  </si>
+  <si>
+    <t>62692</t>
+  </si>
+  <si>
+    <t>60626</t>
+  </si>
+  <si>
+    <t>57975</t>
+  </si>
+  <si>
+    <t>20463</t>
+  </si>
+  <si>
+    <t>72022</t>
+  </si>
+  <si>
+    <t>71998</t>
+  </si>
+  <si>
+    <t>9279</t>
+  </si>
+  <si>
+    <t>64832</t>
+  </si>
+  <si>
+    <t>60589</t>
+  </si>
+  <si>
+    <t>71855</t>
+  </si>
+  <si>
     <t>53038</t>
   </si>
   <si>
-    <t>57307</t>
-  </si>
-  <si>
-    <t>52909</t>
-  </si>
-  <si>
-    <t>62692</t>
+    <t>70807</t>
+  </si>
+  <si>
+    <t>67107</t>
+  </si>
+  <si>
+    <t>8405</t>
   </si>
   <si>
     <t>72043</t>
   </si>
   <si>
-    <t>60626</t>
-  </si>
-  <si>
-    <t>57975</t>
-  </si>
-  <si>
-    <t>72022</t>
-  </si>
-  <si>
-    <t>71998</t>
-  </si>
-  <si>
-    <t>74753</t>
-  </si>
-  <si>
-    <t>64832</t>
-  </si>
-  <si>
-    <t>72002</t>
-  </si>
-  <si>
-    <t>71855</t>
+    <t>48646</t>
+  </si>
+  <si>
+    <t>70950</t>
+  </si>
+  <si>
+    <t>65197</t>
   </si>
   <si>
     <t>46773</t>
   </si>
   <si>
-    <t>73634</t>
-  </si>
-  <si>
-    <t>67107</t>
-  </si>
-  <si>
-    <t>8405</t>
+    <t>72175</t>
   </si>
   <si>
     <t>72917</t>
   </si>
   <si>
-    <t>48646</t>
-  </si>
-  <si>
-    <t>20463</t>
-  </si>
-  <si>
-    <t>70950</t>
-  </si>
-  <si>
-    <t>65197</t>
-  </si>
-  <si>
-    <t>9279</t>
-  </si>
-  <si>
-    <t>70807</t>
-  </si>
-  <si>
-    <t>60589</t>
-  </si>
-  <si>
-    <t>72175</t>
+    <t>43229</t>
   </si>
   <si>
     <t>69831</t>
@@ -198,9 +201,6 @@
     <t>63143</t>
   </si>
   <si>
-    <t>43229</t>
-  </si>
-  <si>
     <t>73375</t>
   </si>
   <si>
@@ -216,33 +216,36 @@
     <t>64314</t>
   </si>
   <si>
+    <t>10936</t>
+  </si>
+  <si>
     <t>67198</t>
   </si>
   <si>
-    <t>10936</t>
-  </si>
-  <si>
     <t>72292</t>
   </si>
   <si>
     <t>72194</t>
   </si>
   <si>
+    <t>57078</t>
+  </si>
+  <si>
+    <t>26983</t>
+  </si>
+  <si>
+    <t>22596</t>
+  </si>
+  <si>
+    <t>53973</t>
+  </si>
+  <si>
+    <t>71136</t>
+  </si>
+  <si>
     <t>18447</t>
   </si>
   <si>
-    <t>26983</t>
-  </si>
-  <si>
-    <t>53973</t>
-  </si>
-  <si>
-    <t>71136</t>
-  </si>
-  <si>
-    <t>22596</t>
-  </si>
-  <si>
     <t>46808</t>
   </si>
   <si>
@@ -255,9 +258,6 @@
     <t>66628</t>
   </si>
   <si>
-    <t>57078</t>
-  </si>
-  <si>
     <t>50843</t>
   </si>
   <si>
@@ -273,133 +273,136 @@
     <t>41359</t>
   </si>
   <si>
+    <t>6836</t>
+  </si>
+  <si>
     <t>36124</t>
   </si>
   <si>
-    <t>6836</t>
-  </si>
-  <si>
     <t>69453</t>
   </si>
   <si>
     <t>49405</t>
   </si>
   <si>
+    <t>2700-134</t>
+  </si>
+  <si>
+    <t>2610-303</t>
+  </si>
+  <si>
+    <t>2720-008</t>
+  </si>
+  <si>
+    <t>2720-203</t>
+  </si>
+  <si>
+    <t>2610-166</t>
+  </si>
+  <si>
+    <t>2700-503</t>
+  </si>
+  <si>
+    <t>2700-778</t>
+  </si>
+  <si>
     <t>2700-320</t>
   </si>
   <si>
-    <t>2720-008</t>
-  </si>
-  <si>
-    <t>2720-203</t>
-  </si>
-  <si>
-    <t>2610-303</t>
-  </si>
-  <si>
-    <t>2700-778</t>
-  </si>
-  <si>
-    <t>2700-134</t>
-  </si>
-  <si>
-    <t>2610-166</t>
-  </si>
-  <si>
-    <t>2700-503</t>
-  </si>
-  <si>
     <t>2775-293</t>
   </si>
   <si>
     <t>1070-132</t>
   </si>
   <si>
+    <t>1070-326</t>
+  </si>
+  <si>
     <t>1150-143</t>
   </si>
   <si>
-    <t>1070-326</t>
+    <t>1200-625</t>
+  </si>
+  <si>
+    <t>1300-049</t>
   </si>
   <si>
     <t>1300-118</t>
   </si>
   <si>
+    <t>1200-030</t>
+  </si>
+  <si>
+    <t>1300-303</t>
+  </si>
+  <si>
+    <t>1300-490</t>
+  </si>
+  <si>
+    <t>1300-514</t>
+  </si>
+  <si>
+    <t>1000-048</t>
+  </si>
+  <si>
+    <t>1070-011</t>
+  </si>
+  <si>
+    <t>1350-344</t>
+  </si>
+  <si>
+    <t>1350-346</t>
+  </si>
+  <si>
+    <t>1400-058</t>
+  </si>
+  <si>
+    <t>1400-118</t>
+  </si>
+  <si>
+    <t>1400-232</t>
+  </si>
+  <si>
+    <t>1990-302</t>
+  </si>
+  <si>
+    <t>1700-175</t>
+  </si>
+  <si>
     <t>1300-275</t>
   </si>
   <si>
-    <t>1200-625</t>
-  </si>
-  <si>
-    <t>1300-049</t>
-  </si>
-  <si>
-    <t>1300-514</t>
+    <t>1800-284</t>
+  </si>
+  <si>
+    <t>1600-067</t>
+  </si>
+  <si>
+    <t>1600-174</t>
   </si>
   <si>
     <t>1300-544</t>
   </si>
   <si>
-    <t>1000-048</t>
-  </si>
-  <si>
-    <t>1070-011</t>
-  </si>
-  <si>
-    <t>1350-346</t>
-  </si>
-  <si>
-    <t>1400-058</t>
-  </si>
-  <si>
-    <t>1200-030</t>
-  </si>
-  <si>
-    <t>1400-232</t>
-  </si>
-  <si>
-    <t>1300-490</t>
-  </si>
-  <si>
-    <t>1700-175</t>
+    <t>1350-226</t>
+  </si>
+  <si>
+    <t>1600-313</t>
+  </si>
+  <si>
+    <t>1600-621</t>
   </si>
   <si>
     <t>1800-268</t>
   </si>
   <si>
-    <t>1300-303</t>
-  </si>
-  <si>
-    <t>1600-067</t>
-  </si>
-  <si>
-    <t>1600-174</t>
+    <t>1500-627</t>
   </si>
   <si>
     <t>1500-442</t>
   </si>
   <si>
-    <t>1350-226</t>
-  </si>
-  <si>
-    <t>1350-344</t>
-  </si>
-  <si>
-    <t>1600-313</t>
-  </si>
-  <si>
-    <t>1600-621</t>
-  </si>
-  <si>
-    <t>1400-118</t>
-  </si>
-  <si>
-    <t>1800-284</t>
-  </si>
-  <si>
-    <t>1990-302</t>
-  </si>
-  <si>
-    <t>1500-627</t>
+    <t>2670-579</t>
   </si>
   <si>
     <t>2660-205</t>
@@ -411,9 +414,6 @@
     <t>2660-287</t>
   </si>
   <si>
-    <t>2670-579</t>
-  </si>
-  <si>
     <t>2640-300</t>
   </si>
   <si>
@@ -429,33 +429,36 @@
     <t>2675-295</t>
   </si>
   <si>
+    <t>2620-396</t>
+  </si>
+  <si>
     <t>2620-458</t>
   </si>
   <si>
-    <t>2620-396</t>
-  </si>
-  <si>
     <t>2675-356</t>
   </si>
   <si>
     <t>2675-242</t>
   </si>
   <si>
+    <t>1495-065</t>
+  </si>
+  <si>
+    <t>1495-038</t>
+  </si>
+  <si>
+    <t>1495-203</t>
+  </si>
+  <si>
+    <t>1495-161</t>
+  </si>
+  <si>
+    <t>2770-113</t>
+  </si>
+  <si>
     <t>1495-097</t>
   </si>
   <si>
-    <t>1495-038</t>
-  </si>
-  <si>
-    <t>1495-161</t>
-  </si>
-  <si>
-    <t>2770-113</t>
-  </si>
-  <si>
-    <t>1495-203</t>
-  </si>
-  <si>
     <t>1495-725</t>
   </si>
   <si>
@@ -468,9 +471,6 @@
     <t>2790-216</t>
   </si>
   <si>
-    <t>1495-065</t>
-  </si>
-  <si>
     <t>2730-201</t>
   </si>
   <si>
@@ -486,10 +486,10 @@
     <t>2745-316</t>
   </si>
   <si>
+    <t>2605-753</t>
+  </si>
+  <si>
     <t>2605-863</t>
-  </si>
-  <si>
-    <t>2605-753</t>
   </si>
   <si>
     <t>2615-164</t>
@@ -1612,16 +1612,16 @@
         <v>43.78</v>
       </c>
       <c r="P2" t="n">
-        <v>7.66</v>
+        <v>7.61</v>
       </c>
       <c r="Q2" t="n">
-        <v>-9.23902958274587</v>
+        <v>-9.227124476677972</v>
       </c>
       <c r="R2" t="n">
-        <v>38.75965669875092</v>
+        <v>38.75402594011345</v>
       </c>
       <c r="S2" t="n">
-        <v>11.9075</v>
+        <v>13.056000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -1671,16 +1671,16 @@
         <v>43.78</v>
       </c>
       <c r="P3" t="n">
-        <v>7.75</v>
+        <v>6.6</v>
       </c>
       <c r="Q3" t="n">
-        <v>-9.219593756877282</v>
+        <v>-9.212092425991159</v>
       </c>
       <c r="R3" t="n">
-        <v>38.74534707730874</v>
+        <v>38.74216670073373</v>
       </c>
       <c r="S3" t="n">
-        <v>12.296833333333332</v>
+        <v>11.4735</v>
       </c>
     </row>
     <row r="4">
@@ -1730,16 +1730,16 @@
         <v>43.78</v>
       </c>
       <c r="P4" t="n">
-        <v>6.96</v>
+        <v>7.75</v>
       </c>
       <c r="Q4" t="n">
-        <v>-9.229045442945981</v>
+        <v>-9.219593756877282</v>
       </c>
       <c r="R4" t="n">
-        <v>38.752286858908015</v>
+        <v>38.74534707730874</v>
       </c>
       <c r="S4" t="n">
-        <v>10.970833333333333</v>
+        <v>12.296833333333332</v>
       </c>
     </row>
     <row r="5">
@@ -1789,16 +1789,16 @@
         <v>43.78</v>
       </c>
       <c r="P5" t="n">
-        <v>6.6</v>
+        <v>6.96</v>
       </c>
       <c r="Q5" t="n">
-        <v>-9.212092425991159</v>
+        <v>-9.229045442945981</v>
       </c>
       <c r="R5" t="n">
-        <v>38.74216670073373</v>
+        <v>38.752286858908015</v>
       </c>
       <c r="S5" t="n">
-        <v>11.4735</v>
+        <v>10.970833333333333</v>
       </c>
     </row>
     <row r="6">
@@ -1848,16 +1848,16 @@
         <v>43.78</v>
       </c>
       <c r="P6" t="n">
-        <v>9.08</v>
+        <v>5.42</v>
       </c>
       <c r="Q6" t="n">
-        <v>-9.23091969121144</v>
+        <v>-9.208425763351675</v>
       </c>
       <c r="R6" t="n">
-        <v>38.767626904837556</v>
+        <v>38.73695837363175</v>
       </c>
       <c r="S6" t="n">
-        <v>14.869833333333334</v>
+        <v>11.909500000000001</v>
       </c>
     </row>
     <row r="7">
@@ -1907,16 +1907,16 @@
         <v>43.78</v>
       </c>
       <c r="P7" t="n">
-        <v>7.61</v>
+        <v>9.33</v>
       </c>
       <c r="Q7" t="n">
-        <v>-9.227124476677972</v>
+        <v>-9.227556119955496</v>
       </c>
       <c r="R7" t="n">
-        <v>38.75402594011345</v>
+        <v>38.7682520642555</v>
       </c>
       <c r="S7" t="n">
-        <v>13.056000000000001</v>
+        <v>15.322833333333334</v>
       </c>
     </row>
     <row r="8">
@@ -1966,16 +1966,16 @@
         <v>43.78</v>
       </c>
       <c r="P8" t="n">
-        <v>5.42</v>
+        <v>9.08</v>
       </c>
       <c r="Q8" t="n">
-        <v>-9.208425763351675</v>
+        <v>-9.23091969121144</v>
       </c>
       <c r="R8" t="n">
-        <v>38.73695837363175</v>
+        <v>38.767626904837556</v>
       </c>
       <c r="S8" t="n">
-        <v>11.909500000000001</v>
+        <v>14.869833333333334</v>
       </c>
     </row>
     <row r="9">
@@ -2025,16 +2025,16 @@
         <v>43.78</v>
       </c>
       <c r="P9" t="n">
-        <v>9.33</v>
+        <v>7.66</v>
       </c>
       <c r="Q9" t="n">
-        <v>-9.227556119955496</v>
+        <v>-9.23902958274587</v>
       </c>
       <c r="R9" t="n">
-        <v>38.7682520642555</v>
+        <v>38.75965669875092</v>
       </c>
       <c r="S9" t="n">
-        <v>15.322833333333334</v>
+        <v>11.9075</v>
       </c>
     </row>
     <row r="10">
@@ -2202,16 +2202,16 @@
         <v>43.78</v>
       </c>
       <c r="P12" t="n">
-        <v>7.88</v>
+        <v>4.84</v>
       </c>
       <c r="Q12" t="n">
-        <v>-9.138124809598237</v>
+        <v>-9.168065103757932</v>
       </c>
       <c r="R12" t="n">
-        <v>38.72490298501254</v>
+        <v>38.72440275922384</v>
       </c>
       <c r="S12" t="n">
-        <v>14.0725</v>
+        <v>8.430166666666667</v>
       </c>
     </row>
     <row r="13">
@@ -2261,16 +2261,16 @@
         <v>43.78</v>
       </c>
       <c r="P13" t="n">
-        <v>4.84</v>
+        <v>7.88</v>
       </c>
       <c r="Q13" t="n">
-        <v>-9.168065103757932</v>
+        <v>-9.138124809598237</v>
       </c>
       <c r="R13" t="n">
-        <v>38.72440275922384</v>
+        <v>38.72490298501254</v>
       </c>
       <c r="S13" t="n">
-        <v>8.430166666666667</v>
+        <v>14.0725</v>
       </c>
     </row>
     <row r="14">
@@ -2320,16 +2320,16 @@
         <v>43.78</v>
       </c>
       <c r="P14" t="n">
-        <v>0.96</v>
+        <v>5.02</v>
       </c>
       <c r="Q14" t="n">
-        <v>-9.193510216960414</v>
+        <v>-9.162464482029266</v>
       </c>
       <c r="R14" t="n">
-        <v>38.70965211640846</v>
+        <v>38.71010432150604</v>
       </c>
       <c r="S14" t="n">
-        <v>3.8345</v>
+        <v>12.518666666666666</v>
       </c>
     </row>
     <row r="15">
@@ -2379,16 +2379,16 @@
         <v>43.78</v>
       </c>
       <c r="P15" t="n">
-        <v>1.71</v>
+        <v>1.37</v>
       </c>
       <c r="Q15" t="n">
-        <v>-9.189716464143316</v>
+        <v>-9.190803116628858</v>
       </c>
       <c r="R15" t="n">
-        <v>38.70059932222034</v>
+        <v>38.70386818976295</v>
       </c>
       <c r="S15" t="n">
-        <v>6.838166666666667</v>
+        <v>5.3395</v>
       </c>
     </row>
     <row r="16">
@@ -2438,16 +2438,16 @@
         <v>43.78</v>
       </c>
       <c r="P16" t="n">
-        <v>5.02</v>
+        <v>0.96</v>
       </c>
       <c r="Q16" t="n">
-        <v>-9.162464482029266</v>
+        <v>-9.193510216960414</v>
       </c>
       <c r="R16" t="n">
-        <v>38.71010432150604</v>
+        <v>38.70965211640846</v>
       </c>
       <c r="S16" t="n">
-        <v>12.518666666666666</v>
+        <v>3.8345</v>
       </c>
     </row>
     <row r="17">
@@ -2497,16 +2497,16 @@
         <v>43.78</v>
       </c>
       <c r="P17" t="n">
-        <v>1.37</v>
+        <v>7.65</v>
       </c>
       <c r="Q17" t="n">
-        <v>-9.190803116628858</v>
+        <v>-9.149150413715839</v>
       </c>
       <c r="R17" t="n">
-        <v>38.70386818976295</v>
+        <v>38.71377349224416</v>
       </c>
       <c r="S17" t="n">
-        <v>5.3395</v>
+        <v>15.292</v>
       </c>
     </row>
     <row r="18">
@@ -2556,16 +2556,16 @@
         <v>43.78</v>
       </c>
       <c r="P18" t="n">
-        <v>1.97</v>
+        <v>2.33</v>
       </c>
       <c r="Q18" t="n">
-        <v>-9.186315852092283</v>
+        <v>-9.182503399120106</v>
       </c>
       <c r="R18" t="n">
-        <v>38.70271446067282</v>
+        <v>38.705299736027</v>
       </c>
       <c r="S18" t="n">
-        <v>7.014833333333333</v>
+        <v>7.376166666666666</v>
       </c>
     </row>
     <row r="19">
@@ -2615,16 +2615,16 @@
         <v>43.78</v>
       </c>
       <c r="P19" t="n">
-        <v>2.65</v>
+        <v>1.57</v>
       </c>
       <c r="Q19" t="n">
-        <v>-9.177038612926374</v>
+        <v>-9.192235202736674</v>
       </c>
       <c r="R19" t="n">
-        <v>38.706513245579345</v>
+        <v>38.70131157737532</v>
       </c>
       <c r="S19" t="n">
-        <v>7.741</v>
+        <v>6.268833333333333</v>
       </c>
     </row>
     <row r="20">
@@ -2674,16 +2674,16 @@
         <v>43.78</v>
       </c>
       <c r="P20" t="n">
-        <v>8.84</v>
+        <v>1.97</v>
       </c>
       <c r="Q20" t="n">
-        <v>-9.134219849847394</v>
+        <v>-9.186315852092283</v>
       </c>
       <c r="R20" t="n">
-        <v>38.7354983295513</v>
+        <v>38.70271446067282</v>
       </c>
       <c r="S20" t="n">
-        <v>14.581</v>
+        <v>7.014833333333333</v>
       </c>
     </row>
     <row r="21">
@@ -2733,16 +2733,16 @@
         <v>43.78</v>
       </c>
       <c r="P21" t="n">
-        <v>6.04</v>
+        <v>8.84</v>
       </c>
       <c r="Q21" t="n">
-        <v>-9.171475268225077</v>
+        <v>-9.134219849847394</v>
       </c>
       <c r="R21" t="n">
-        <v>38.73166512300516</v>
+        <v>38.7354983295513</v>
       </c>
       <c r="S21" t="n">
-        <v>11.731333333333334</v>
+        <v>14.581</v>
       </c>
     </row>
     <row r="22">
@@ -2792,16 +2792,16 @@
         <v>43.78</v>
       </c>
       <c r="P22" t="n">
-        <v>4.11</v>
+        <v>6.04</v>
       </c>
       <c r="Q22" t="n">
-        <v>-9.163991607578955</v>
+        <v>-9.171475268225077</v>
       </c>
       <c r="R22" t="n">
-        <v>38.703725895399565</v>
+        <v>38.73166512300516</v>
       </c>
       <c r="S22" t="n">
-        <v>10.2585</v>
+        <v>11.731333333333334</v>
       </c>
     </row>
     <row r="23">
@@ -2851,16 +2851,16 @@
         <v>43.78</v>
       </c>
       <c r="P23" t="n">
-        <v>1.09</v>
+        <v>3.39</v>
       </c>
       <c r="Q23" t="n">
-        <v>-9.204469520005299</v>
+        <v>-9.173405803619335</v>
       </c>
       <c r="R23" t="n">
-        <v>38.712580795464426</v>
+        <v>38.70534230115484</v>
       </c>
       <c r="S23" t="n">
-        <v>3.8266666666666667</v>
+        <v>9.538333333333332</v>
       </c>
     </row>
     <row r="24">
@@ -2910,16 +2910,16 @@
         <v>43.78</v>
       </c>
       <c r="P24" t="n">
-        <v>7.65</v>
+        <v>4.11</v>
       </c>
       <c r="Q24" t="n">
-        <v>-9.149150413715839</v>
+        <v>-9.163991607578955</v>
       </c>
       <c r="R24" t="n">
-        <v>38.71377349224416</v>
+        <v>38.703725895399565</v>
       </c>
       <c r="S24" t="n">
-        <v>15.292</v>
+        <v>10.2585</v>
       </c>
     </row>
     <row r="25">
@@ -2969,16 +2969,16 @@
         <v>43.78</v>
       </c>
       <c r="P25" t="n">
-        <v>1.54</v>
+        <v>1.09</v>
       </c>
       <c r="Q25" t="n">
-        <v>-9.207052340111456</v>
+        <v>-9.204469520005299</v>
       </c>
       <c r="R25" t="n">
-        <v>38.712755612094384</v>
+        <v>38.712580795464426</v>
       </c>
       <c r="S25" t="n">
-        <v>5.203333333333333</v>
+        <v>3.8266666666666667</v>
       </c>
     </row>
     <row r="26">
@@ -3028,16 +3028,16 @@
         <v>43.78</v>
       </c>
       <c r="P26" t="n">
-        <v>1.57</v>
+        <v>4.34</v>
       </c>
       <c r="Q26" t="n">
-        <v>-9.192235202736674</v>
+        <v>-9.21518662202578</v>
       </c>
       <c r="R26" t="n">
-        <v>38.70131157737532</v>
+        <v>38.699331369461355</v>
       </c>
       <c r="S26" t="n">
-        <v>6.268833333333333</v>
+        <v>8.9485</v>
       </c>
     </row>
     <row r="27">
@@ -3087,16 +3087,16 @@
         <v>43.78</v>
       </c>
       <c r="P27" t="n">
-        <v>10.23</v>
+        <v>1.54</v>
       </c>
       <c r="Q27" t="n">
-        <v>-9.135803152303748</v>
+        <v>-9.207052340111456</v>
       </c>
       <c r="R27" t="n">
-        <v>38.749098171383714</v>
+        <v>38.712755612094384</v>
       </c>
       <c r="S27" t="n">
-        <v>16.743166666666667</v>
+        <v>5.203333333333333</v>
       </c>
     </row>
     <row r="28">
@@ -3146,16 +3146,16 @@
         <v>43.78</v>
       </c>
       <c r="P28" t="n">
-        <v>14.8</v>
+        <v>17.3</v>
       </c>
       <c r="Q28" t="n">
-        <v>-9.108469625466748</v>
+        <v>-9.094964764177647</v>
       </c>
       <c r="R28" t="n">
-        <v>38.762010709657126</v>
+        <v>38.78036758202002</v>
       </c>
       <c r="S28" t="n">
-        <v>23.227333333333334</v>
+        <v>26.081</v>
       </c>
     </row>
     <row r="29">
@@ -3205,16 +3205,16 @@
         <v>43.78</v>
       </c>
       <c r="P29" t="n">
-        <v>2.33</v>
+        <v>10.23</v>
       </c>
       <c r="Q29" t="n">
-        <v>-9.182503399120106</v>
+        <v>-9.135803152303748</v>
       </c>
       <c r="R29" t="n">
-        <v>38.705299736027</v>
+        <v>38.749098171383714</v>
       </c>
       <c r="S29" t="n">
-        <v>7.376166666666666</v>
+        <v>16.743166666666667</v>
       </c>
     </row>
     <row r="30">
@@ -3264,16 +3264,16 @@
         <v>43.78</v>
       </c>
       <c r="P30" t="n">
-        <v>11.47</v>
+        <v>1.71</v>
       </c>
       <c r="Q30" t="n">
-        <v>-9.17019590540944</v>
+        <v>-9.189716464143316</v>
       </c>
       <c r="R30" t="n">
-        <v>38.76971898281831</v>
+        <v>38.70059932222034</v>
       </c>
       <c r="S30" t="n">
-        <v>19.829333333333334</v>
+        <v>6.838166666666667</v>
       </c>
     </row>
     <row r="31">
@@ -3323,16 +3323,16 @@
         <v>43.78</v>
       </c>
       <c r="P31" t="n">
-        <v>7.95</v>
+        <v>13.86</v>
       </c>
       <c r="Q31" t="n">
-        <v>-9.167451582796662</v>
+        <v>-9.118832111842389</v>
       </c>
       <c r="R31" t="n">
-        <v>38.74800512929091</v>
+        <v>38.770323153566316</v>
       </c>
       <c r="S31" t="n">
-        <v>14.911</v>
+        <v>23.694166666666668</v>
       </c>
     </row>
     <row r="32">
@@ -3382,16 +3382,16 @@
         <v>43.78</v>
       </c>
       <c r="P32" t="n">
-        <v>9.48</v>
+        <v>11.47</v>
       </c>
       <c r="Q32" t="n">
-        <v>-9.1862199879522</v>
+        <v>-9.17019590540944</v>
       </c>
       <c r="R32" t="n">
-        <v>38.748336624709324</v>
+        <v>38.76971898281831</v>
       </c>
       <c r="S32" t="n">
-        <v>17.217499999999998</v>
+        <v>19.829333333333334</v>
       </c>
     </row>
     <row r="33">
@@ -3441,16 +3441,16 @@
         <v>43.78</v>
       </c>
       <c r="P33" t="n">
-        <v>6.57</v>
+        <v>7.95</v>
       </c>
       <c r="Q33" t="n">
-        <v>-9.168744494418952</v>
+        <v>-9.167451582796662</v>
       </c>
       <c r="R33" t="n">
-        <v>38.71555987953703</v>
+        <v>38.74800512929091</v>
       </c>
       <c r="S33" t="n">
-        <v>12.2855</v>
+        <v>14.911</v>
       </c>
     </row>
     <row r="34">
@@ -3500,16 +3500,16 @@
         <v>43.78</v>
       </c>
       <c r="P34" t="n">
-        <v>3.39</v>
+        <v>2.65</v>
       </c>
       <c r="Q34" t="n">
-        <v>-9.173405803619335</v>
+        <v>-9.177038612926374</v>
       </c>
       <c r="R34" t="n">
-        <v>38.70534230115484</v>
+        <v>38.706513245579345</v>
       </c>
       <c r="S34" t="n">
-        <v>9.538333333333332</v>
+        <v>7.741</v>
       </c>
     </row>
     <row r="35">
@@ -3559,16 +3559,16 @@
         <v>43.78</v>
       </c>
       <c r="P35" t="n">
-        <v>8.59</v>
+        <v>6.57</v>
       </c>
       <c r="Q35" t="n">
-        <v>-9.152979279613735</v>
+        <v>-9.168744494418952</v>
       </c>
       <c r="R35" t="n">
-        <v>38.74649422360284</v>
+        <v>38.71555987953703</v>
       </c>
       <c r="S35" t="n">
-        <v>14.671</v>
+        <v>12.2855</v>
       </c>
     </row>
     <row r="36">
@@ -3618,16 +3618,16 @@
         <v>43.78</v>
       </c>
       <c r="P36" t="n">
-        <v>11.67</v>
+        <v>8.59</v>
       </c>
       <c r="Q36" t="n">
-        <v>-9.168933075659652</v>
+        <v>-9.152979279613735</v>
       </c>
       <c r="R36" t="n">
-        <v>38.77151315617074</v>
+        <v>38.74649422360284</v>
       </c>
       <c r="S36" t="n">
-        <v>19.977333333333334</v>
+        <v>14.671</v>
       </c>
     </row>
     <row r="37">
@@ -3677,16 +3677,16 @@
         <v>43.78</v>
       </c>
       <c r="P37" t="n">
-        <v>4.34</v>
+        <v>11.67</v>
       </c>
       <c r="Q37" t="n">
-        <v>-9.21518662202578</v>
+        <v>-9.168933075659652</v>
       </c>
       <c r="R37" t="n">
-        <v>38.699331369461355</v>
+        <v>38.77151315617074</v>
       </c>
       <c r="S37" t="n">
-        <v>8.9485</v>
+        <v>19.977333333333334</v>
       </c>
     </row>
     <row r="38">
@@ -3736,16 +3736,16 @@
         <v>43.78</v>
       </c>
       <c r="P38" t="n">
-        <v>13.86</v>
+        <v>14.8</v>
       </c>
       <c r="Q38" t="n">
-        <v>-9.118832111842389</v>
+        <v>-9.108469625466748</v>
       </c>
       <c r="R38" t="n">
-        <v>38.770323153566316</v>
+        <v>38.762010709657126</v>
       </c>
       <c r="S38" t="n">
-        <v>23.694166666666668</v>
+        <v>23.227333333333334</v>
       </c>
     </row>
     <row r="39">
@@ -3795,16 +3795,16 @@
         <v>43.78</v>
       </c>
       <c r="P39" t="n">
-        <v>17.3</v>
+        <v>9.72</v>
       </c>
       <c r="Q39" t="n">
-        <v>-9.094964764177647</v>
+        <v>-9.180542249269829</v>
       </c>
       <c r="R39" t="n">
-        <v>38.78036758202002</v>
+        <v>38.75234234899489</v>
       </c>
       <c r="S39" t="n">
-        <v>26.081</v>
+        <v>17.268166666666666</v>
       </c>
     </row>
     <row r="40">
@@ -3854,16 +3854,16 @@
         <v>43.78</v>
       </c>
       <c r="P40" t="n">
-        <v>9.72</v>
+        <v>9.48</v>
       </c>
       <c r="Q40" t="n">
-        <v>-9.180542249269829</v>
+        <v>-9.1862199879522</v>
       </c>
       <c r="R40" t="n">
-        <v>38.75234234899489</v>
+        <v>38.748336624709324</v>
       </c>
       <c r="S40" t="n">
-        <v>17.268166666666666</v>
+        <v>17.217499999999998</v>
       </c>
     </row>
     <row r="41">
@@ -3913,16 +3913,16 @@
         <v>43.78</v>
       </c>
       <c r="P41" t="n">
-        <v>18.31</v>
+        <v>21.08</v>
       </c>
       <c r="Q41" t="n">
-        <v>-9.1784201940559</v>
+        <v>-9.156355972200505</v>
       </c>
       <c r="R41" t="n">
-        <v>38.811871544844514</v>
+        <v>38.839654133437186</v>
       </c>
       <c r="S41" t="n">
-        <v>22.427333333333333</v>
+        <v>24.1245</v>
       </c>
     </row>
     <row r="42">
@@ -3972,16 +3972,16 @@
         <v>43.78</v>
       </c>
       <c r="P42" t="n">
-        <v>15.62</v>
+        <v>18.31</v>
       </c>
       <c r="Q42" t="n">
-        <v>-9.162975046794587</v>
+        <v>-9.1784201940559</v>
       </c>
       <c r="R42" t="n">
-        <v>38.78577658465522</v>
+        <v>38.811871544844514</v>
       </c>
       <c r="S42" t="n">
-        <v>23.584333333333333</v>
+        <v>22.427333333333333</v>
       </c>
     </row>
     <row r="43">
@@ -4031,16 +4031,16 @@
         <v>43.78</v>
       </c>
       <c r="P43" t="n">
-        <v>17.85</v>
+        <v>15.62</v>
       </c>
       <c r="Q43" t="n">
-        <v>-9.16141808470935</v>
+        <v>-9.162975046794587</v>
       </c>
       <c r="R43" t="n">
-        <v>38.815024580815724</v>
+        <v>38.78577658465522</v>
       </c>
       <c r="S43" t="n">
-        <v>21.582666666666668</v>
+        <v>23.584333333333333</v>
       </c>
     </row>
     <row r="44">
@@ -4090,16 +4090,16 @@
         <v>43.78</v>
       </c>
       <c r="P44" t="n">
-        <v>21.08</v>
+        <v>17.85</v>
       </c>
       <c r="Q44" t="n">
-        <v>-9.156355972200505</v>
+        <v>-9.16141808470935</v>
       </c>
       <c r="R44" t="n">
-        <v>38.839654133437186</v>
+        <v>38.815024580815724</v>
       </c>
       <c r="S44" t="n">
-        <v>24.1245</v>
+        <v>21.582666666666668</v>
       </c>
     </row>
     <row r="45">
@@ -4444,16 +4444,16 @@
         <v>43.78</v>
       </c>
       <c r="P50" t="n">
-        <v>16.22</v>
+        <v>17.62</v>
       </c>
       <c r="Q50" t="n">
-        <v>-9.191285825930667</v>
+        <v>-9.195209120267327</v>
       </c>
       <c r="R50" t="n">
-        <v>38.80587187819032</v>
+        <v>38.81114362352943</v>
       </c>
       <c r="S50" t="n">
-        <v>21.255166666666664</v>
+        <v>21.745833333333334</v>
       </c>
     </row>
     <row r="51">
@@ -4503,16 +4503,16 @@
         <v>43.78</v>
       </c>
       <c r="P51" t="n">
-        <v>17.62</v>
+        <v>16.22</v>
       </c>
       <c r="Q51" t="n">
-        <v>-9.195209120267327</v>
+        <v>-9.191285825930667</v>
       </c>
       <c r="R51" t="n">
-        <v>38.81114362352943</v>
+        <v>38.80587187819032</v>
       </c>
       <c r="S51" t="n">
-        <v>21.745833333333334</v>
+        <v>21.255166666666664</v>
       </c>
     </row>
     <row r="52">
@@ -4680,16 +4680,16 @@
         <v>43.78</v>
       </c>
       <c r="P54" t="n">
-        <v>7.61</v>
+        <v>6.82</v>
       </c>
       <c r="Q54" t="n">
-        <v>-9.232874587724558</v>
+        <v>-9.229158315654166</v>
       </c>
       <c r="R54" t="n">
-        <v>38.702751475538136</v>
+        <v>38.708248127846936</v>
       </c>
       <c r="S54" t="n">
-        <v>12.030333333333335</v>
+        <v>10.384833333333335</v>
       </c>
     </row>
     <row r="55">
@@ -4798,16 +4798,16 @@
         <v>43.78</v>
       </c>
       <c r="P56" t="n">
-        <v>7.01</v>
+        <v>7.32</v>
       </c>
       <c r="Q56" t="n">
-        <v>-9.227267787420203</v>
+        <v>-9.230025848172497</v>
       </c>
       <c r="R56" t="n">
-        <v>38.713253175837714</v>
+        <v>38.70389825245811</v>
       </c>
       <c r="S56" t="n">
-        <v>10.679666666666666</v>
+        <v>11.058666666666666</v>
       </c>
     </row>
     <row r="57">
@@ -4857,16 +4857,16 @@
         <v>43.78</v>
       </c>
       <c r="P57" t="n">
-        <v>15.21</v>
+        <v>7.01</v>
       </c>
       <c r="Q57" t="n">
-        <v>-9.30184160776297</v>
+        <v>-9.227267787420203</v>
       </c>
       <c r="R57" t="n">
-        <v>38.691421690918524</v>
+        <v>38.713253175837714</v>
       </c>
       <c r="S57" t="n">
-        <v>17.601666666666667</v>
+        <v>10.679666666666666</v>
       </c>
     </row>
     <row r="58">
@@ -4916,16 +4916,16 @@
         <v>43.78</v>
       </c>
       <c r="P58" t="n">
-        <v>7.32</v>
+        <v>15.21</v>
       </c>
       <c r="Q58" t="n">
-        <v>-9.230025848172497</v>
+        <v>-9.30184160776297</v>
       </c>
       <c r="R58" t="n">
-        <v>38.70389825245811</v>
+        <v>38.691421690918524</v>
       </c>
       <c r="S58" t="n">
-        <v>11.058666666666666</v>
+        <v>17.601666666666667</v>
       </c>
     </row>
     <row r="59">
@@ -4975,16 +4975,16 @@
         <v>43.78</v>
       </c>
       <c r="P59" t="n">
-        <v>10.88</v>
+        <v>7.61</v>
       </c>
       <c r="Q59" t="n">
-        <v>-9.24020674721426</v>
+        <v>-9.232874587724558</v>
       </c>
       <c r="R59" t="n">
-        <v>38.69930377427593</v>
+        <v>38.702751475538136</v>
       </c>
       <c r="S59" t="n">
-        <v>12.355666666666668</v>
+        <v>12.030333333333335</v>
       </c>
     </row>
     <row r="60">
@@ -5034,16 +5034,16 @@
         <v>43.78</v>
       </c>
       <c r="P60" t="n">
-        <v>10.42</v>
+        <v>10.88</v>
       </c>
       <c r="Q60" t="n">
-        <v>-9.260143396654147</v>
+        <v>-9.24020674721426</v>
       </c>
       <c r="R60" t="n">
-        <v>38.71686165833169</v>
+        <v>38.69930377427593</v>
       </c>
       <c r="S60" t="n">
-        <v>12.009666666666668</v>
+        <v>12.355666666666668</v>
       </c>
     </row>
     <row r="61">
@@ -5093,16 +5093,16 @@
         <v>43.78</v>
       </c>
       <c r="P61" t="n">
-        <v>7.48</v>
+        <v>10.42</v>
       </c>
       <c r="Q61" t="n">
-        <v>-9.235527426629362</v>
+        <v>-9.260143396654147</v>
       </c>
       <c r="R61" t="n">
-        <v>38.72669361676505</v>
+        <v>38.71686165833169</v>
       </c>
       <c r="S61" t="n">
-        <v>11.197833333333334</v>
+        <v>12.009666666666668</v>
       </c>
     </row>
     <row r="62">
@@ -5152,16 +5152,16 @@
         <v>43.78</v>
       </c>
       <c r="P62" t="n">
-        <v>5.49</v>
+        <v>7.48</v>
       </c>
       <c r="Q62" t="n">
-        <v>-9.226158352325164</v>
+        <v>-9.235527426629362</v>
       </c>
       <c r="R62" t="n">
-        <v>38.720992271268834</v>
+        <v>38.72669361676505</v>
       </c>
       <c r="S62" t="n">
-        <v>11.614666666666666</v>
+        <v>11.197833333333334</v>
       </c>
     </row>
     <row r="63">
@@ -5211,16 +5211,16 @@
         <v>43.78</v>
       </c>
       <c r="P63" t="n">
-        <v>6.82</v>
+        <v>5.49</v>
       </c>
       <c r="Q63" t="n">
-        <v>-9.229158315654166</v>
+        <v>-9.226158352325164</v>
       </c>
       <c r="R63" t="n">
-        <v>38.708248127846936</v>
+        <v>38.720992271268834</v>
       </c>
       <c r="S63" t="n">
-        <v>10.384833333333335</v>
+        <v>11.614666666666666</v>
       </c>
     </row>
     <row r="64">
@@ -5565,16 +5565,16 @@
         <v>43.78</v>
       </c>
       <c r="P69" t="n">
-        <v>14.09</v>
+        <v>15.58</v>
       </c>
       <c r="Q69" t="n">
-        <v>-9.225488245306195</v>
+        <v>-9.231569429491191</v>
       </c>
       <c r="R69" t="n">
-        <v>38.80315601123324</v>
+        <v>38.806039522991014</v>
       </c>
       <c r="S69" t="n">
-        <v>22.652833333333334</v>
+        <v>21.080499999999997</v>
       </c>
     </row>
     <row r="70">
@@ -5624,16 +5624,16 @@
         <v>43.78</v>
       </c>
       <c r="P70" t="n">
-        <v>15.58</v>
+        <v>14.09</v>
       </c>
       <c r="Q70" t="n">
-        <v>-9.231569429491191</v>
+        <v>-9.225488245306195</v>
       </c>
       <c r="R70" t="n">
-        <v>38.806039522991014</v>
+        <v>38.80315601123324</v>
       </c>
       <c r="S70" t="n">
-        <v>21.080499999999997</v>
+        <v>22.652833333333334</v>
       </c>
     </row>
     <row r="71">
@@ -5752,65 +5752,6 @@
       </c>
       <c r="S72" t="n">
         <v>31.762833333333333</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="s">
-        <v>59</v>
-      </c>
-      <c r="B73" t="s">
-        <v>130</v>
-      </c>
-      <c r="C73" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D73" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E73" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F73" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G73" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H73" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I73" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J73" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K73" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L73" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M73" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N73" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O73" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="P73" t="n">
-        <v>15.62</v>
-      </c>
-      <c r="Q73" t="n">
-        <v>-9.162975046794587</v>
-      </c>
-      <c r="R73" t="n">
-        <v>38.78577658465522</v>
-      </c>
-      <c r="S73" t="n">
-        <v>23.584333333333333</v>
       </c>
     </row>
   </sheetData>
@@ -8309,7 +8250,7 @@
         <v>218</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C43" t="s">
         <v>163</v>
@@ -9784,7 +9725,7 @@
         <v>243</v>
       </c>
       <c r="B68" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C68" t="s">
         <v>163</v>

</xml_diff>